<commit_message>
Fixed economics using excel evaluations
</commit_message>
<xml_diff>
--- a/explanatory_notes/Evaluations.xlsx
+++ b/explanatory_notes/Evaluations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>План реализации копий ПО</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Годовая прибыль</t>
+  </si>
+  <si>
+    <t>Рентабильность затрат на разраб.</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -166,12 +169,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E47"/>
+  <dimension ref="A2:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,130 +565,134 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>800</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <f>B6/B2/8</f>
         <v>4.7393364928909953</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>460</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <f>C6*D6</f>
         <v>2180.0947867298578</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>800</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <f>B7/B2/8</f>
         <v>4.7393364928909953</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>80</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <f t="shared" ref="E7:E9" si="0">C7*D7</f>
         <v>379.14691943127963</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>800</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <f>B8/B2/8</f>
         <v>4.7393364928909953</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>80</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>379.14691943127963</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>600</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <f>B9/B2/8</f>
         <v>3.5545023696682461</v>
       </c>
-      <c r="D9">
-        <v>56</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="1">
+        <v>160</v>
+      </c>
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>199.05213270142178</v>
+        <v>568.72037914691941</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10">
-        <f>D6+D7+D8+D9</f>
-        <v>676</v>
-      </c>
-      <c r="E10">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3">
         <f>E6+E7+E8+E9</f>
-        <v>3137.4407582938384</v>
+        <v>3507.1090047393363</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>50</v>
       </c>
-      <c r="E11">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3">
         <f>E10*(B11/100)</f>
-        <v>1568.7203791469192</v>
+        <v>1753.5545023696682</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E12">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4">
         <f>E10+E11</f>
-        <v>4706.1611374407576</v>
+        <v>5260.6635071090041</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -624,7 +709,7 @@
       </c>
       <c r="B15">
         <f>E12*(B14/100)</f>
-        <v>941.23222748815158</v>
+        <v>1052.1327014218009</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -641,7 +726,7 @@
       </c>
       <c r="B18">
         <f>(E12+B15)*(B17/100)</f>
-        <v>1976.5876777251181</v>
+        <v>2209.4786729857815</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -658,7 +743,7 @@
       </c>
       <c r="B21">
         <f>E12*(B20/100)</f>
-        <v>4706.1611374407576</v>
+        <v>5260.6635071090041</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -667,7 +752,7 @@
       </c>
       <c r="B23">
         <f>E12+B15+B18+B21</f>
-        <v>12330.142180094785</v>
+        <v>13782.938388625591</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -676,7 +761,7 @@
       </c>
       <c r="B25">
         <f>B23*0.05</f>
-        <v>616.50710900473928</v>
+        <v>689.14691943127957</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -685,7 +770,7 @@
       </c>
       <c r="B26">
         <f>B25+B23</f>
-        <v>12946.649289099523</v>
+        <v>14472.08530805687</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +778,7 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -702,7 +787,7 @@
       </c>
       <c r="B29">
         <f>(B26*B28)/(B3*100)</f>
-        <v>107.88874407582935</v>
+        <v>80.400473933649295</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +796,7 @@
       </c>
       <c r="B30">
         <f>B26/B3+B29</f>
-        <v>467.51789099526059</v>
+        <v>482.40284360189571</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -720,202 +805,190 @@
       </c>
       <c r="B31">
         <f>B29*B3</f>
-        <v>3883.9947867298565</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+        <v>2894.4170616113747</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32">
+        <f>B31/B26*100</f>
+        <v>20.000000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>8</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>0.18</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B35">
+      <c r="B36" s="4">
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C36" s="4">
         <v>1</v>
       </c>
-      <c r="D35">
+      <c r="D36" s="4">
         <v>2</v>
       </c>
-      <c r="E35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B36">
+      <c r="B37" s="4">
         <v>24</v>
       </c>
-      <c r="C36">
+      <c r="C37" s="4">
         <f>B3</f>
         <v>36</v>
       </c>
-      <c r="D36">
+      <c r="D37" s="4">
         <f>B3</f>
         <v>36</v>
       </c>
-      <c r="E36">
-        <f>B3</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B37">
-        <f>B36*B30</f>
-        <v>11220.429383886254</v>
-      </c>
-      <c r="C37">
-        <f>C36*B30</f>
-        <v>16830.644075829383</v>
-      </c>
-      <c r="D37">
-        <f>D36*B30</f>
-        <v>16830.644075829383</v>
-      </c>
-      <c r="E37">
-        <f>E36*B30</f>
-        <v>16830.644075829383</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="B38" s="4">
+        <f>B37*B30</f>
+        <v>11577.668246445497</v>
+      </c>
+      <c r="C38" s="4">
+        <f>C37*B30</f>
+        <v>17366.502369668247</v>
+      </c>
+      <c r="D38" s="4">
+        <f>D37*B30</f>
+        <v>17366.502369668247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B38">
-        <f>B37*B45</f>
-        <v>11220.429383886254</v>
-      </c>
-      <c r="C38">
-        <f>C37*C45</f>
-        <v>14263.257691380833</v>
-      </c>
-      <c r="D38">
-        <f>D37*D45</f>
-        <v>12087.506518119351</v>
-      </c>
-      <c r="E38">
-        <f>E37*E45</f>
-        <v>10243.649591626569</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="B39" s="4">
+        <f>B38*B46</f>
+        <v>11577.668246445497</v>
+      </c>
+      <c r="C39" s="4">
+        <f>C38*C46</f>
+        <v>14717.374889549363</v>
+      </c>
+      <c r="D39" s="4">
+        <f>D38*D46</f>
+        <v>12472.351601313019</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B40">
+      <c r="B41" s="4">
         <f>B26</f>
-        <v>12946.649289099523</v>
-      </c>
-      <c r="C40">
+        <v>14472.08530805687</v>
+      </c>
+      <c r="C41" s="4">
         <v>0</v>
       </c>
-      <c r="D40">
+      <c r="D41" s="4">
         <v>0</v>
       </c>
-      <c r="E40">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="4">
+        <f>B41*B46</f>
+        <v>14472.08530805687</v>
+      </c>
+      <c r="C42" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41">
-        <f>B40*B45</f>
-        <v>12946.649289099523</v>
-      </c>
-      <c r="C41">
+      <c r="D42" s="4">
         <v>0</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B43">
-        <f>B38-B41</f>
-        <v>-1726.2199052132692</v>
-      </c>
-      <c r="C43">
-        <f>C38-C41</f>
-        <v>14263.257691380833</v>
-      </c>
-      <c r="D43">
-        <f>D38-D41</f>
-        <v>12087.506518119351</v>
-      </c>
-      <c r="E43">
-        <f>E38-E41</f>
-        <v>10243.649591626569</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="B44" s="4">
+        <f>B39-B42</f>
+        <v>-2894.4170616113734</v>
+      </c>
+      <c r="C44" s="4">
+        <f>C39-C42</f>
+        <v>14717.374889549363</v>
+      </c>
+      <c r="D44" s="4">
+        <f>D39-D42</f>
+        <v>12472.351601313019</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B44">
-        <f>B45*B43</f>
-        <v>-1726.2199052132692</v>
-      </c>
-      <c r="C44">
-        <f>C43+B44</f>
-        <v>12537.037786167564</v>
-      </c>
-      <c r="D44">
-        <f>D43+C44</f>
-        <v>24624.544304286916</v>
-      </c>
-      <c r="E44">
-        <f>E43+D44</f>
-        <v>34868.193895913486</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B45" s="4">
+        <f>B46*B44</f>
+        <v>-2894.4170616113734</v>
+      </c>
+      <c r="C45" s="4">
+        <f>C44+B45</f>
+        <v>11822.957827937989</v>
+      </c>
+      <c r="D45" s="4">
+        <f>D44+C45</f>
+        <v>24295.309429251007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B45">
-        <f>1/POWER(1+B33,B35 )</f>
+      <c r="B46" s="4">
+        <f>1/POWER(1+B34,B36 )</f>
         <v>1</v>
       </c>
-      <c r="C45">
-        <f>1/POWER(1+B33,C35 )</f>
+      <c r="C46" s="4">
+        <f>1/POWER(1+B34,C36 )</f>
         <v>0.84745762711864414</v>
       </c>
-      <c r="D45">
-        <f>1/POWER(1+B33,D35 )</f>
+      <c r="D46" s="4">
+        <f>1/POWER(1+B34,D36 )</f>
         <v>0.71818442976156283</v>
       </c>
-      <c r="E45">
-        <f>1/POWER(1+B33,E35 )</f>
-        <v>0.6086308726792905</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>10</v>
       </c>
-      <c r="B47">
-        <f>(E44/B41)*100</f>
-        <v>269.32214750940142</v>
+      <c r="B48">
+        <f>(D45/B42)*100</f>
+        <v>167.87704682562486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>